<commit_message>
Sales_Analytics  & Customer_Analytics & Store_Analytics & Product_Analytics
</commit_message>
<xml_diff>
--- a/batches/21/week_06_analytics_final_project/day_17/day_17.xlsx
+++ b/batches/21/week_06_analytics_final_project/day_17/day_17.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shira/Documents/modules/sql/batches/21/week_06_analytics_final_project/day_17/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2C7492E-3AA5-8C4A-AC7D-C53AD0C50FB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAB745A2-9220-ED40-9056-9139930B16F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="1" xr2:uid="{853FB50E-7653-4943-859A-B1D787894A4C}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="2" xr2:uid="{853FB50E-7653-4943-859A-B1D787894A4C}"/>
   </bookViews>
   <sheets>
     <sheet name="Recap" sheetId="1" r:id="rId1"/>
     <sheet name="Agenda" sheetId="2" r:id="rId2"/>
+    <sheet name="Project" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="128">
   <si>
     <t>📚 COMPREHENSIVE RECAP (Days 1-16)</t>
   </si>
@@ -370,6 +371,57 @@
   </si>
   <si>
     <t>&amp;&amp; touch "RetailMart Analytics Project"/06_documentation/{data_dictionary.md,kpi_definitions.md}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Schema </t>
+  </si>
+  <si>
+    <t>Metadata</t>
+  </si>
+  <si>
+    <t>Sales Analytics</t>
+  </si>
+  <si>
+    <t>Monthly Sales Dashboard with Trends</t>
+  </si>
+  <si>
+    <t>Daily Sales Summary</t>
+  </si>
+  <si>
+    <t>Sales by Day of Week Analytics</t>
+  </si>
+  <si>
+    <t>Hourly Sales Pattern</t>
+  </si>
+  <si>
+    <t>Sales by Payment Mode</t>
+  </si>
+  <si>
+    <t>Sales Vs Returns Analysis</t>
+  </si>
+  <si>
+    <t>Quarterly Sales Performance</t>
+  </si>
+  <si>
+    <t>Export Data for Dashboard</t>
+  </si>
+  <si>
+    <t>Product Analytics</t>
+  </si>
+  <si>
+    <t>Top Products Performance</t>
+  </si>
+  <si>
+    <t>Category Performance Analysis</t>
+  </si>
+  <si>
+    <t>Brand Performance Analysis</t>
+  </si>
+  <si>
+    <t>ABC Analysis (Parento 80-20)</t>
+  </si>
+  <si>
+    <t>Inventory Turnover Analysis</t>
   </si>
 </sst>
 </file>
@@ -1186,7 +1238,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{60518233-54B1-7248-8496-2388CF6E5AB1}">
   <dimension ref="B2:F35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="212" workbookViewId="0">
+    <sheetView topLeftCell="A18" zoomScale="212" workbookViewId="0">
       <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
@@ -1357,4 +1409,109 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E6C0615-7612-5C49-BB98-3A0FBD5E6603}">
+  <dimension ref="B2:C20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="248" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="3.1640625" customWidth="1"/>
+    <col min="2" max="2" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B5" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="C6" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="C7" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="C8" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="9" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="C9" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="10" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="C10" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="11" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="C11" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="12" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="C12" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="C13" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="15" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="16" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="C16" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="17" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C17" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="18" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C18" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="19" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C19" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="20" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C20" t="s">
+        <v>127</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Project Ready for Production
</commit_message>
<xml_diff>
--- a/batches/21/week_06_analytics_final_project/day_17/day_17.xlsx
+++ b/batches/21/week_06_analytics_final_project/day_17/day_17.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/shira/Documents/modules/sql/batches/21/week_06_analytics_final_project/day_17/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAB745A2-9220-ED40-9056-9139930B16F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F51EB2B6-2E7C-DA41-AEEB-23DC818995E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="2" xr2:uid="{853FB50E-7653-4943-859A-B1D787894A4C}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" activeTab="3" xr2:uid="{853FB50E-7653-4943-859A-B1D787894A4C}"/>
   </bookViews>
   <sheets>
     <sheet name="Recap" sheetId="1" r:id="rId1"/>
     <sheet name="Agenda" sheetId="2" r:id="rId2"/>
     <sheet name="Project" sheetId="3" r:id="rId3"/>
+    <sheet name="Flow Chart" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="134">
   <si>
     <t>📚 COMPREHENSIVE RECAP (Days 1-16)</t>
   </si>
@@ -382,46 +383,64 @@
     <t>Sales Analytics</t>
   </si>
   <si>
-    <t>Monthly Sales Dashboard with Trends</t>
-  </si>
-  <si>
-    <t>Daily Sales Summary</t>
-  </si>
-  <si>
-    <t>Sales by Day of Week Analytics</t>
-  </si>
-  <si>
-    <t>Hourly Sales Pattern</t>
-  </si>
-  <si>
-    <t>Sales by Payment Mode</t>
-  </si>
-  <si>
-    <t>Sales Vs Returns Analysis</t>
-  </si>
-  <si>
-    <t>Quarterly Sales Performance</t>
-  </si>
-  <si>
-    <t>Export Data for Dashboard</t>
-  </si>
-  <si>
     <t>Product Analytics</t>
   </si>
   <si>
-    <t>Top Products Performance</t>
-  </si>
-  <si>
-    <t>Category Performance Analysis</t>
-  </si>
-  <si>
-    <t>Brand Performance Analysis</t>
-  </si>
-  <si>
-    <t>ABC Analysis (Parento 80-20)</t>
-  </si>
-  <si>
-    <t>Inventory Turnover Analysis</t>
+    <t>Retailmart Database</t>
+  </si>
+  <si>
+    <t>8 Schemas</t>
+  </si>
+  <si>
+    <t>analytics</t>
+  </si>
+  <si>
+    <t>customers</t>
+  </si>
+  <si>
+    <t>sales</t>
+  </si>
+  <si>
+    <t>stores</t>
+  </si>
+  <si>
+    <t>products</t>
+  </si>
+  <si>
+    <t>kpi</t>
+  </si>
+  <si>
+    <t>trends</t>
+  </si>
+  <si>
+    <t>monthly / weekly / yearly</t>
+  </si>
+  <si>
+    <t>Customer_anlytics.sql</t>
+  </si>
+  <si>
+    <t>Views</t>
+  </si>
+  <si>
+    <t>Materialized Views</t>
+  </si>
+  <si>
+    <t>refresh_procedure</t>
+  </si>
+  <si>
+    <t>function convert our data into json files</t>
+  </si>
+  <si>
+    <t>Front End</t>
+  </si>
+  <si>
+    <t>style.css</t>
+  </si>
+  <si>
+    <t>Execute these Functions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">.json </t>
   </si>
 </sst>
 </file>
@@ -1413,10 +1432,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E6C0615-7612-5C49-BB98-3A0FBD5E6603}">
-  <dimension ref="B2:C20"/>
+  <dimension ref="B2:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="248" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView zoomScale="248" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1426,89 +1445,140 @@
     <col min="3" max="3" width="31.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="C6" t="s">
+    <row r="15" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>114</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E421C366-2357-2443-9950-5E8230ABA7C0}">
+  <dimension ref="B2:H18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="227" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="32.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="3.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="C7" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="C8" t="s">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="C3" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="C9" t="s">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="C4" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="C10" t="s">
+      <c r="D4" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="C11" t="s">
+      <c r="F4" t="s">
+        <v>122</v>
+      </c>
+      <c r="G4" t="s">
+        <v>123</v>
+      </c>
+      <c r="H4" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="D5" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="12" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="C12" t="s">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="D6" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="13" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="C13" t="s">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="D7" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B15" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="C16" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C17" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C18" t="s">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="D10" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C19" t="s">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="E11" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="20" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C20" t="s">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="E12" t="s">
         <v>127</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="E13" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="E14" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="H15" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="E16" t="s">
+        <v>132</v>
+      </c>
+      <c r="H16" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="17" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="E17" t="s">
+        <v>133</v>
+      </c>
+      <c r="H17" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="18" spans="5:8" x14ac:dyDescent="0.2">
+      <c r="H18" t="s">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>